<commit_message>
remove useless discipline form controls
</commit_message>
<xml_diff>
--- a/src/test/resources/parser/bachelor.xlsx
+++ b/src/test/resources/parser/bachelor.xlsx
@@ -1,26 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\hneu-personal-account\src\test\resources\parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oleksandrrozdolskyi/Repos/hneu-personal-account/src/test/resources/parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10995"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="11000"/>
   </bookViews>
   <sheets>
     <sheet name="БАКАЛАВР" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">БАКАЛАВР!$A$1:$K$75</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">БАКАЛАВР!$15:$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">БАКАЛАВР!$A$1:$K$75</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
   <si>
     <t>Декан факультету</t>
   </si>
@@ -55,9 +61,6 @@
   </si>
   <si>
     <t>МАЙНОР 3 або ВІЛЬНИЙ МАЙНОР 3</t>
-  </si>
-  <si>
-    <t>Диф. залік</t>
   </si>
   <si>
     <t>VІ СЕМЕСТР</t>
@@ -227,9 +230,6 @@
     <t>Розподілені та паралельні обчислення</t>
   </si>
   <si>
-    <t>ЗВІТ</t>
-  </si>
-  <si>
     <t>Захист інформації</t>
   </si>
   <si>
@@ -259,9 +259,6 @@
     <t>Державний екзамен з іноземної мови</t>
   </si>
   <si>
-    <t>Держ. Екзамен</t>
-  </si>
-  <si>
     <t>Дипломний проект</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
   </si>
   <si>
     <t>Операційні системи</t>
-  </si>
-  <si>
-    <t>Курсовий проект</t>
   </si>
   <si>
     <t xml:space="preserve">Теорія інформації і кодування </t>
@@ -354,15 +348,18 @@
   <si>
     <t>mopis101@gmail.com</t>
   </si>
+  <si>
+    <t>Залік</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,8 +547,31 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,6 +590,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -582,11 +608,11 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,25 +621,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -621,7 +647,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -630,59 +656,59 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -691,67 +717,67 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -760,18 +786,18 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -779,37 +805,38 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -952,75 +979,450 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="84">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1298,7 +1700,7 @@
         <xdr:cNvPr id="2" name="Группа 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1307,7 +1709,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11480205" cy="1357312"/>
+          <a:ext cx="13016111" cy="1349374"/>
           <a:chOff x="10633" y="6"/>
           <a:chExt cx="7649775" cy="854145"/>
         </a:xfrm>
@@ -1317,7 +1719,7 @@
           <xdr:cNvPr id="3" name="Рисунок 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1350,7 +1752,7 @@
           <xdr:cNvPr id="4" name="Рисунок 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1383,7 +1785,7 @@
           <xdr:cNvPr id="5" name="Прямоугольник 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1714,7 +2116,7 @@
         <xdr:cNvPr id="6" name="Прямоугольник 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1780,7 +2182,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2074,213 +2476,213 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A57" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A60" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.42578125" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="0.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="45.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="0.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="0.6640625" style="1" customWidth="1"/>
     <col min="13" max="14" width="30" style="1" customWidth="1"/>
-    <col min="15" max="15" width="53.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="48.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="17.42578125" style="1"/>
+    <col min="15" max="15" width="53.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="48.6640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="17.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-    </row>
-    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+    <row r="1" spans="1:11" ht="84.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:11" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+    </row>
+    <row r="4" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+    </row>
+    <row r="5" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-    </row>
-    <row r="5" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="43" t="s">
+      <c r="C6" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+    </row>
+    <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+    </row>
+    <row r="9" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="63">
+        <v>2016</v>
+      </c>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+    </row>
+    <row r="11" spans="1:11" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+    </row>
+    <row r="12" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="41"/>
+      <c r="C12" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-    </row>
-    <row r="7" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-    </row>
-    <row r="8" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-    </row>
-    <row r="9" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="59">
-        <v>2016</v>
-      </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-    </row>
-    <row r="11" spans="1:11" s="42" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-    </row>
-    <row r="12" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="41"/>
-      <c r="C12" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-    </row>
-    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="62" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+    </row>
+    <row r="13" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
       <c r="K13" s="40"/>
     </row>
-    <row r="14" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
+        <v>69</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
     </row>
-    <row r="15" spans="1:11" s="14" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="14" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="H15" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="I15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="37" t="s">
-        <v>21</v>
-      </c>
       <c r="J15" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" s="36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="14" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="14" customFormat="1" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="16"/>
       <c r="C16" s="30"/>
@@ -2292,67 +2694,67 @@
       <c r="J16" s="30"/>
       <c r="K16" s="29"/>
     </row>
-    <row r="17" spans="1:11" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="53"/>
-    </row>
-    <row r="18" spans="1:11" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
+    <row r="17" spans="1:11" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="G18" s="55" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="54"/>
+    </row>
+    <row r="18" spans="1:11" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-    </row>
-    <row r="19" spans="1:11" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="58" t="s">
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="G18" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="55"/>
+    </row>
+    <row r="19" spans="1:11" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="26"/>
-      <c r="G19" s="48" t="s">
+      <c r="G19" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="50"/>
-    </row>
-    <row r="20" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="58"/>
+    </row>
+    <row r="20" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23">
         <f>IF(B20=0,0,1)</f>
         <v>1</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="21">
         <v>1</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E20" s="19"/>
       <c r="G20" s="20">
@@ -2360,29 +2762,29 @@
         <v>1</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I20" s="21">
         <v>5</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K20" s="27"/>
     </row>
-    <row r="21" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23">
         <f t="shared" ref="A21:A23" si="0">IF(B21=0,0,A20+1)</f>
         <v>2</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C21" s="21">
         <v>4</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E21" s="19"/>
       <c r="G21" s="20">
@@ -2390,29 +2792,29 @@
         <v>2</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I21" s="21">
         <v>5</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" s="27"/>
     </row>
-    <row r="22" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="21">
         <v>5</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" s="19"/>
       <c r="G22" s="20">
@@ -2420,29 +2822,29 @@
         <v>3</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I22" s="21">
         <v>5</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" s="27"/>
     </row>
-    <row r="23" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="21">
         <v>4</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E23" s="19"/>
       <c r="G23" s="20">
@@ -2450,29 +2852,29 @@
         <v>4</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I23" s="21">
         <v>5</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" s="27"/>
     </row>
-    <row r="24" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23">
         <f>IF(B24=0,0,A23+1)</f>
         <v>5</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="21">
         <v>7</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="19"/>
       <c r="G24" s="20">
@@ -2480,73 +2882,73 @@
         <v>5</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="21">
         <v>4</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K24" s="27"/>
     </row>
-    <row r="25" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="23">
         <v>6</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="21">
         <v>4</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E25" s="19"/>
       <c r="G25" s="20">
         <v>6</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I25" s="21">
         <v>4</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K25" s="27"/>
     </row>
-    <row r="26" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="23">
         <v>7</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="21">
         <v>5</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="19"/>
       <c r="G26" s="20">
         <v>7</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I26" s="21">
         <v>2</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K26" s="27"/>
     </row>
-    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <f>IF(B27=0,0,#REF!+1)</f>
         <v>0</v>
@@ -2561,7 +2963,7 @@
       <c r="I27" s="16"/>
       <c r="K27" s="15"/>
     </row>
-    <row r="28" spans="1:11" s="8" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="8" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="12" t="str">
         <f>CONCATENATE("ВСЬОГО ЗА ",A18)</f>
@@ -2586,7 +2988,7 @@
       <c r="J28" s="10"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" s="14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" s="14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="16"/>
       <c r="C29" s="30"/>
@@ -2598,67 +3000,67 @@
       <c r="J29" s="30"/>
       <c r="K29" s="29"/>
     </row>
-    <row r="30" spans="1:11" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="53"/>
-    </row>
-    <row r="31" spans="1:11" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+    <row r="30" spans="1:11" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="G31" s="55" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="56"/>
-    </row>
-    <row r="32" spans="1:11" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="58" t="s">
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="54"/>
+    </row>
+    <row r="31" spans="1:11" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="G31" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="55"/>
+    </row>
+    <row r="32" spans="1:11" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
       <c r="F32" s="26"/>
-      <c r="G32" s="48" t="s">
+      <c r="G32" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="48"/>
-      <c r="I32" s="48"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="50"/>
-    </row>
-    <row r="33" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="57"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="57"/>
+      <c r="K32" s="58"/>
+    </row>
+    <row r="33" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="23">
         <f>IF(B33=0,0,1)</f>
         <v>1</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="21">
         <v>5</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="19"/>
       <c r="G33" s="20">
@@ -2666,29 +3068,29 @@
         <v>1</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I33" s="21">
         <v>5</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K33" s="27"/>
     </row>
-    <row r="34" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="23">
         <f>IF(B34=0,0,A33+1)</f>
         <v>2</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="21">
         <v>4</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E34" s="19"/>
       <c r="G34" s="20">
@@ -2696,29 +3098,29 @@
         <v>2</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I34" s="21">
         <v>4</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K34" s="27"/>
     </row>
-    <row r="35" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="23">
         <f>IF(B35=0,0,A34+1)</f>
         <v>3</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="21">
         <v>5</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="19"/>
       <c r="G35" s="20">
@@ -2726,29 +3128,29 @@
         <v>3</v>
       </c>
       <c r="H35" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I35" s="21">
         <v>5</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K35" s="27"/>
     </row>
-    <row r="36" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="23">
         <f>IF(B36=0,0,A35+1)</f>
         <v>4</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="21">
         <v>7</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" s="19"/>
       <c r="G36" s="20">
@@ -2756,13 +3158,13 @@
         <v>4</v>
       </c>
       <c r="H36" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I36" s="21">
         <v>6</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K36" s="27"/>
       <c r="L36" s="45"/>
@@ -2770,32 +3172,32 @@
       <c r="N36" s="45"/>
       <c r="O36" s="45"/>
     </row>
-    <row r="37" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="23">
         <f>IF(B37=0,0,A36+1)</f>
         <v>5</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C37" s="21">
         <v>4</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E37" s="19"/>
       <c r="G37" s="20">
         <v>5</v>
       </c>
       <c r="H37" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I37" s="21">
         <v>1</v>
       </c>
       <c r="J37" s="20" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="K37" s="27"/>
       <c r="L37" s="45"/>
@@ -2803,39 +3205,39 @@
       <c r="N37" s="45"/>
       <c r="O37" s="45"/>
     </row>
-    <row r="38" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G38" s="20">
         <v>6</v>
       </c>
       <c r="H38" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I38" s="21">
         <v>4</v>
       </c>
       <c r="J38" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K38" s="27"/>
     </row>
-    <row r="39" spans="1:16" s="14" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
+    <row r="39" spans="1:16" s="14" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
       <c r="F39" s="26"/>
-      <c r="G39" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="H39" s="57"/>
-      <c r="I39" s="57"/>
-      <c r="J39" s="57"/>
-      <c r="K39" s="57"/>
-    </row>
-    <row r="40" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+    </row>
+    <row r="40" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="33">
         <f>IF(B40=0,0,MAX(A33:A37)+1)</f>
         <v>0</v>
@@ -2845,7 +3247,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E40" s="19"/>
       <c r="G40" s="32">
@@ -2857,14 +3259,14 @@
         <v>5</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K40" s="27"/>
       <c r="M40" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N40" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O40" s="34" t="s">
         <v>6</v>
@@ -2873,7 +3275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="14" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="14" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <f>IF(B41=0,0,#REF!+1)</f>
         <v>0</v>
@@ -2888,7 +3290,7 @@
       <c r="I41" s="16"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:16" s="8" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" s="8" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="12" t="str">
         <f>CONCATENATE("ВСЬОГО ЗА ",A31)</f>
@@ -2913,7 +3315,7 @@
       <c r="J42" s="10"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:16" s="14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" s="14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="29"/>
       <c r="B43" s="16"/>
       <c r="C43" s="30"/>
@@ -2925,67 +3327,67 @@
       <c r="J43" s="30"/>
       <c r="K43" s="29"/>
     </row>
-    <row r="44" spans="1:16" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="53"/>
-    </row>
-    <row r="45" spans="1:16" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="54" t="s">
+    <row r="44" spans="1:16" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="G45" s="55" t="s">
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="54"/>
+    </row>
+    <row r="45" spans="1:16" s="14" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="56"/>
-    </row>
-    <row r="46" spans="1:16" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="58" t="s">
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="G45" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="55"/>
+    </row>
+    <row r="46" spans="1:16" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
       <c r="F46" s="26"/>
-      <c r="G46" s="48" t="s">
+      <c r="G46" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="50"/>
-    </row>
-    <row r="47" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="57"/>
+      <c r="K46" s="58"/>
+    </row>
+    <row r="47" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="23">
         <f>IF(B47=0,0,1)</f>
         <v>1</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="21">
         <v>7</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E47" s="19"/>
       <c r="G47" s="20">
@@ -2993,29 +3395,29 @@
         <v>1</v>
       </c>
       <c r="H47" s="28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I47" s="21">
         <v>4</v>
       </c>
       <c r="J47" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K47" s="27"/>
     </row>
-    <row r="48" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="23">
         <f>IF(B48=0,0,A47+1)</f>
         <v>2</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="21">
         <v>5</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E48" s="19"/>
       <c r="G48" s="20">
@@ -3023,29 +3425,29 @@
         <v>2</v>
       </c>
       <c r="H48" s="28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I48" s="21">
         <v>5</v>
       </c>
       <c r="J48" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K48" s="27"/>
     </row>
-    <row r="49" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="23">
         <f>IF(B49=0,0,A48+1)</f>
         <v>3</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C49" s="21">
         <v>4</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E49" s="19"/>
       <c r="G49" s="20">
@@ -3053,52 +3455,52 @@
         <v>3</v>
       </c>
       <c r="H49" s="28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I49" s="21">
         <v>1</v>
       </c>
       <c r="J49" s="20" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="K49" s="27"/>
     </row>
-    <row r="50" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23">
         <f>IF(B50=0,0,A49+1)</f>
         <v>4</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="21">
         <v>5</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E50" s="19"/>
-      <c r="G50" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="H50" s="49"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="50"/>
-    </row>
-    <row r="51" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G50" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="H50" s="68"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="58"/>
+    </row>
+    <row r="51" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
         <f>IF(B51=0,0,A50+1)</f>
         <v>5</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C51" s="21">
         <v>2</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="E51" s="19"/>
       <c r="G51" s="32">
@@ -3110,40 +3512,40 @@
         <v>5</v>
       </c>
       <c r="J51" s="20" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="K51" s="27"/>
     </row>
-    <row r="52" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
         <v>6</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C52" s="21">
         <v>2</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E52" s="19"/>
-      <c r="G52" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52" s="57"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-    </row>
-    <row r="53" spans="1:16" s="14" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
+      <c r="G52" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+    </row>
+    <row r="53" spans="1:16" s="14" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
       <c r="F53" s="26"/>
       <c r="G53" s="32">
         <f>IF(H53=0,0,G51+1)</f>
@@ -3154,11 +3556,11 @@
         <v>5</v>
       </c>
       <c r="J53" s="20" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="K53" s="27"/>
     </row>
-    <row r="54" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="33">
         <f>IF(B54=0,0,MAX(A47:A51)+1)</f>
         <v>0</v>
@@ -3168,7 +3570,7 @@
         <v>5</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E54" s="19"/>
       <c r="G54" s="32">
@@ -3180,7 +3582,7 @@
         <v>5</v>
       </c>
       <c r="J54" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K54" s="27"/>
       <c r="M54" s="24" t="s">
@@ -3196,12 +3598,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="54"/>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
+    <row r="55" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="49"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
       <c r="G55" s="32">
         <f>IF(H55=0,0,G54+1)</f>
         <v>0</v>
@@ -3211,7 +3613,7 @@
         <v>5</v>
       </c>
       <c r="J55" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K55" s="27"/>
       <c r="M55" s="24"/>
@@ -3219,7 +3621,7 @@
       <c r="O55" s="34"/>
       <c r="P55" s="35"/>
     </row>
-    <row r="56" spans="1:16" s="14" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="14" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="12" t="str">
         <f>CONCATENATE("ВСЬОГО ЗА ",A45)</f>
@@ -3244,7 +3646,7 @@
       <c r="J56" s="10"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="1:16" s="14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" s="14" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="29"/>
       <c r="B57" s="16"/>
       <c r="C57" s="30"/>
@@ -3256,67 +3658,67 @@
       <c r="J57" s="30"/>
       <c r="K57" s="29"/>
     </row>
-    <row r="58" spans="1:16" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="51" t="s">
+    <row r="58" spans="1:16" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="52"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="52"/>
-      <c r="G58" s="52"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="53"/>
-    </row>
-    <row r="59" spans="1:16" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="54" t="s">
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="54"/>
+    </row>
+    <row r="59" spans="1:16" s="14" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
-      <c r="G59" s="55" t="s">
+      <c r="B59" s="50"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="G59" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="56"/>
-    </row>
-    <row r="60" spans="1:16" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="58" t="s">
+      <c r="H59" s="50"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="50"/>
+      <c r="K59" s="55"/>
+    </row>
+    <row r="60" spans="1:16" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="57"/>
       <c r="F60" s="26"/>
-      <c r="G60" s="48" t="s">
+      <c r="G60" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
-      <c r="K60" s="50"/>
-    </row>
-    <row r="61" spans="1:16" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="57"/>
+      <c r="I60" s="57"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="58"/>
+    </row>
+    <row r="61" spans="1:16" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="23">
         <f>IF(B61=0,0,1)</f>
         <v>1</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C61" s="21">
         <v>5</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E61" s="19"/>
       <c r="G61" s="20">
@@ -3324,29 +3726,29 @@
         <v>1</v>
       </c>
       <c r="H61" s="28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I61" s="21">
         <v>2</v>
       </c>
       <c r="J61" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="K61" s="27"/>
     </row>
-    <row r="62" spans="1:16" s="14" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="14" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="23">
         <f>IF(B62=0,0,A61+1)</f>
         <v>2</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C62" s="21">
         <v>5</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E62" s="19"/>
       <c r="G62" s="20">
@@ -3354,28 +3756,28 @@
         <v>2</v>
       </c>
       <c r="H62" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I62" s="21">
         <v>3</v>
       </c>
       <c r="J62" s="20" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="K62" s="27"/>
     </row>
-    <row r="63" spans="1:16" s="14" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="14" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="23">
         <v>3</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C63" s="21">
         <v>5</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E63" s="19"/>
       <c r="G63" s="20">
@@ -3383,28 +3785,28 @@
         <v>3</v>
       </c>
       <c r="H63" s="28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I63" s="21">
         <v>5</v>
       </c>
       <c r="J63" s="20" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="K63" s="27"/>
     </row>
-    <row r="64" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23">
         <v>3</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C64" s="21">
         <v>5</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E64" s="19"/>
       <c r="G64" s="20">
@@ -3412,54 +3814,54 @@
         <v>4</v>
       </c>
       <c r="H64" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I64" s="21">
         <v>2</v>
       </c>
       <c r="J64" s="20" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="K64" s="27"/>
     </row>
-    <row r="65" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="54"/>
-      <c r="B65" s="55"/>
-      <c r="C65" s="55"/>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55"/>
+    <row r="65" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="49"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
       <c r="G65" s="20">
         <v>5</v>
       </c>
       <c r="H65" s="28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I65" s="21">
         <v>8</v>
       </c>
       <c r="J65" s="20" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="K65" s="27"/>
     </row>
-    <row r="66" spans="1:11" s="14" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="B66" s="57"/>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="57"/>
+    <row r="66" spans="1:11" s="14" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="51"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
       <c r="F66" s="26"/>
-      <c r="G66" s="57" t="s">
-        <v>82</v>
-      </c>
-      <c r="H66" s="57"/>
-      <c r="I66" s="57"/>
-      <c r="J66" s="57"/>
-      <c r="K66" s="57"/>
-    </row>
-    <row r="67" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G66" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="51"/>
+    </row>
+    <row r="67" spans="1:11" s="14" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="23">
         <f>IF(B67=0,0,MAX(A61:A65)+1)</f>
         <v>0</v>
@@ -3469,7 +3871,7 @@
         <v>5</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E67" s="19"/>
       <c r="G67" s="32">
@@ -3481,11 +3883,11 @@
         <v>5</v>
       </c>
       <c r="J67" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K67" s="27"/>
     </row>
-    <row r="68" spans="1:11" s="14" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" s="14" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="23">
         <f>IF(B68=0,0,A67+1)</f>
         <v>0</v>
@@ -3494,8 +3896,8 @@
       <c r="C68" s="21">
         <v>5</v>
       </c>
-      <c r="D68" s="20" t="s">
-        <v>9</v>
+      <c r="D68" s="69" t="s">
+        <v>85</v>
       </c>
       <c r="E68" s="19"/>
       <c r="G68" s="32">
@@ -3507,11 +3909,11 @@
         <v>5</v>
       </c>
       <c r="J68" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K68" s="27"/>
     </row>
-    <row r="69" spans="1:11" s="14" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" s="14" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="12" t="str">
         <f>CONCATENATE("ВСЬОГО ЗА ",A59)</f>
@@ -3536,7 +3938,7 @@
       <c r="J69" s="10"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="1:11" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="14" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3549,7 +3951,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" spans="1:11" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="8" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3562,26 +3964,26 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="7">
         <f ca="1">TODAY(  )</f>
-        <v>42813</v>
-      </c>
-      <c r="C72" s="68" t="str">
+        <v>43009</v>
+      </c>
+      <c r="C72" s="48" t="str">
         <f>CONCATENATE("_________________________",LEFT(C7,1)&amp;". ",C6)</f>
         <v>_________________________О. Скороход</v>
       </c>
-      <c r="D72" s="68"/>
-      <c r="E72" s="68"/>
-      <c r="F72" s="68"/>
-      <c r="G72" s="68"/>
-      <c r="H72" s="68"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="48"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
       <c r="B73" s="6"/>
       <c r="C73" s="3"/>
@@ -3594,26 +3996,26 @@
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
     </row>
-    <row r="74" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="6" t="s">
         <v>0</v>
       </c>
       <c r="G74" s="4"/>
     </row>
-    <row r="75" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="6" t="str">
         <f>CONCATENATE(C9," ___________________________________________")</f>
         <v>Економічної інформатики ___________________________________________</v>
       </c>
       <c r="G75" s="4"/>
       <c r="H75" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="1:11" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -3626,7 +4028,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" spans="1:11" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="3" customFormat="1" ht="23" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -3641,18 +4043,22 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="C72:H72"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="G66:K66"/>
-    <mergeCell ref="G52:K52"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="G59:K59"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="G60:K60"/>
-    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="G50:K50"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C8:H8"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="G39:K39"/>
     <mergeCell ref="A18:E18"/>
@@ -3668,175 +4074,247 @@
     <mergeCell ref="A17:K17"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="G32:K32"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="G50:K50"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="G45:K45"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="G46:K46"/>
+    <mergeCell ref="G52:K52"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="G59:K59"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="G60:K60"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="C72:H72"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="G66:K66"/>
   </mergeCells>
-  <conditionalFormatting sqref="D50:D51 J65 D20:D26">
-    <cfRule type="cellIs" dxfId="30" priority="47" operator="equal">
+  <phoneticPr fontId="24" type="noConversion"/>
+  <conditionalFormatting sqref="D20:D26 D50:D51 J65">
+    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J20:J26">
-    <cfRule type="cellIs" dxfId="29" priority="46" operator="equal">
+  <conditionalFormatting sqref="J20:J23">
+    <cfRule type="cellIs" dxfId="82" priority="70" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33:D37">
-    <cfRule type="cellIs" dxfId="28" priority="45" operator="equal">
+  <conditionalFormatting sqref="D33 D35:D36">
+    <cfRule type="cellIs" dxfId="81" priority="69" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33:J36">
-    <cfRule type="cellIs" dxfId="27" priority="44" operator="equal">
+  <conditionalFormatting sqref="J33 J35:J36">
+    <cfRule type="cellIs" dxfId="80" priority="68" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47">
-    <cfRule type="cellIs" dxfId="26" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="60" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J61:J64">
-    <cfRule type="cellIs" dxfId="25" priority="37" operator="equal">
+  <conditionalFormatting sqref="J64">
+    <cfRule type="cellIs" dxfId="78" priority="61" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="cellIs" dxfId="24" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="cellIs" dxfId="23" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="66" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48:D49">
-    <cfRule type="cellIs" dxfId="22" priority="41" operator="equal">
+  <conditionalFormatting sqref="D48">
+    <cfRule type="cellIs" dxfId="75" priority="65" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D67">
+    <cfRule type="cellIs" dxfId="72" priority="57" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B67:B68 H51 H53:H54">
+    <cfRule type="cellIs" dxfId="70" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:H6">
+    <cfRule type="cellIs" dxfId="69" priority="54" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:H7 C8">
+    <cfRule type="cellIs" dxfId="68" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="cellIs" dxfId="67" priority="48" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="cellIs" dxfId="66" priority="47" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="cellIs" dxfId="65" priority="42" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H67">
+    <cfRule type="cellIs" dxfId="63" priority="36" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68">
+    <cfRule type="cellIs" dxfId="62" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J67">
+    <cfRule type="cellIs" dxfId="61" priority="34" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
+    <cfRule type="cellIs" dxfId="57" priority="30" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J68">
+    <cfRule type="cellIs" dxfId="55" priority="27" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H55">
+    <cfRule type="cellIs" dxfId="54" priority="26" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J24">
+    <cfRule type="cellIs" dxfId="49" priority="24" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26">
+    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J37">
+    <cfRule type="cellIs" dxfId="41" priority="20" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="37" priority="18" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40">
+    <cfRule type="cellIs" dxfId="33" priority="16" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J48">
-    <cfRule type="cellIs" dxfId="21" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49">
-    <cfRule type="cellIs" dxfId="20" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D67:D68">
-    <cfRule type="cellIs" dxfId="19" priority="33" operator="equal">
+  <conditionalFormatting sqref="D49">
+    <cfRule type="cellIs" dxfId="25" priority="12" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J51">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J53">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J54">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J55">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"Екзамен"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="cellIs" dxfId="18" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:B68 H51 H53:H54">
-    <cfRule type="cellIs" dxfId="17" priority="31" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:H6">
-    <cfRule type="cellIs" dxfId="16" priority="30" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:H7 C8">
-    <cfRule type="cellIs" dxfId="15" priority="29" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54">
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J54">
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+  <conditionalFormatting sqref="D64">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H67">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H68">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J67">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+  <conditionalFormatting sqref="J61">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J37">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+  <conditionalFormatting sqref="J62">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J38">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"Екзамен"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"Екзамен"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"Екзамен"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"Екзамен"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J68">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Екзамен"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J55">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="J63">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Екзамен"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>